<commit_message>
Correcciones 07, 06 y 05 - Termine en 07 de Facundo Rivero
</commit_message>
<xml_diff>
--- a/Desafios.xlsx
+++ b/Desafios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Boot_80973\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583DFBC3-28C8-477C-8BC9-684B72678837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D253F65-47A3-49C1-8911-119BD7A20F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Ejercicio 4</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Facundo Rivero</t>
-  </si>
-  <si>
-    <t>Tiene que darme acceso a su drive</t>
   </si>
 </sst>
 </file>
@@ -116,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,12 +123,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,17 +165,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +455,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F4" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.88671875" defaultRowHeight="28.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -490,7 +477,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -513,7 +500,7 @@
     </row>
     <row r="5" spans="2:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -530,14 +517,12 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C10" s="7"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="11"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>